<commit_message>
241104, food modified 2
</commit_message>
<xml_diff>
--- a/R/data/food_plan_241104.xlsx
+++ b/R/data/food_plan_241104.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C64DE4-6882-7749-A099-01B158FBE582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C1E89C-1B33-0F48-AAF5-B78C9E1BEEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="377">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -836,6 +836,321 @@
   </si>
   <si>
     <t>이다혜</t>
+  </si>
+  <si>
+    <t>kwonseoyoung0923@gmail.com</t>
+  </si>
+  <si>
+    <t>권서영</t>
+  </si>
+  <si>
+    <t>ystop061012@naver.com</t>
+  </si>
+  <si>
+    <t>미래융합스쿨</t>
+  </si>
+  <si>
+    <t>손연수</t>
+  </si>
+  <si>
+    <t>minheart7844@gmail.com</t>
+  </si>
+  <si>
+    <t>권민</t>
+  </si>
+  <si>
+    <t>rhkwp0323@gmail.com</t>
+  </si>
+  <si>
+    <t>콘텐츠IT</t>
+  </si>
+  <si>
+    <t>유도영</t>
+  </si>
+  <si>
+    <t>sws62550100@gmail.com</t>
+  </si>
+  <si>
+    <t>서우성</t>
+  </si>
+  <si>
+    <t>ckswo00@gmail.com</t>
+  </si>
+  <si>
+    <t>빅데이터</t>
+  </si>
+  <si>
+    <t>이찬재</t>
+  </si>
+  <si>
+    <t>schoe357@gmail.com</t>
+  </si>
+  <si>
+    <t>인공지능융합학부</t>
+  </si>
+  <si>
+    <t>최성민</t>
+  </si>
+  <si>
+    <t>dabinchoe05@gmail.com</t>
+  </si>
+  <si>
+    <t>최다빈</t>
+  </si>
+  <si>
+    <t>ju0_park@naver.com</t>
+  </si>
+  <si>
+    <t>콘텐츠it</t>
+  </si>
+  <si>
+    <t>박주영</t>
+  </si>
+  <si>
+    <t>alwnd816@gmail.com</t>
+  </si>
+  <si>
+    <t>한재은</t>
+  </si>
+  <si>
+    <t>jiteh9491@gmail.com</t>
+  </si>
+  <si>
+    <t>한지예</t>
+  </si>
+  <si>
+    <t>joazzzzz@naver.com</t>
+  </si>
+  <si>
+    <t>빅데이터전공</t>
+  </si>
+  <si>
+    <t>김진구</t>
+  </si>
+  <si>
+    <t>hsjenny99@gmail.com</t>
+  </si>
+  <si>
+    <t>전소현</t>
+  </si>
+  <si>
+    <t>znfh527gkfn@naver.com</t>
+  </si>
+  <si>
+    <t>조준연</t>
+  </si>
+  <si>
+    <t>hug60600@gmail.com</t>
+  </si>
+  <si>
+    <t>황의건</t>
+  </si>
+  <si>
+    <t>cold050317@gmail.com</t>
+  </si>
+  <si>
+    <t>김찬종</t>
+  </si>
+  <si>
+    <t>rivernine369@naver.com</t>
+  </si>
+  <si>
+    <t>강재구</t>
+  </si>
+  <si>
+    <t>corsica2001@naver.com</t>
+  </si>
+  <si>
+    <t>경제학과</t>
+  </si>
+  <si>
+    <t>박상우</t>
+  </si>
+  <si>
+    <t>aone7537@naver.com</t>
+  </si>
+  <si>
+    <t>박현진</t>
+  </si>
+  <si>
+    <t>kter0506@naver.com</t>
+  </si>
+  <si>
+    <t>김태은</t>
+  </si>
+  <si>
+    <t>cjfghksznszns1100119@naver.com</t>
+  </si>
+  <si>
+    <t>유철환</t>
+  </si>
+  <si>
+    <t>bagj11532@gmail.com</t>
+  </si>
+  <si>
+    <t>박준형</t>
+  </si>
+  <si>
+    <t>zorotod@naver.com</t>
+  </si>
+  <si>
+    <t>김승욱</t>
+  </si>
+  <si>
+    <t>syw050819@naver.com</t>
+  </si>
+  <si>
+    <t>신예원</t>
+  </si>
+  <si>
+    <t>bin_1014@naver.com</t>
+  </si>
+  <si>
+    <t>디지털미디어콘텐츠 전공</t>
+  </si>
+  <si>
+    <t>김명빈</t>
+  </si>
+  <si>
+    <t>taehwankim05@gmail.com</t>
+  </si>
+  <si>
+    <t>김태환</t>
+  </si>
+  <si>
+    <t>slaim7888@gmail.com</t>
+  </si>
+  <si>
+    <t>이준민</t>
+  </si>
+  <si>
+    <t>ohsolbi050521@gmail.com</t>
+  </si>
+  <si>
+    <t>오솔비</t>
+  </si>
+  <si>
+    <t>efgh124@naver.com</t>
+  </si>
+  <si>
+    <t>정윤서</t>
+  </si>
+  <si>
+    <t>herdy2154@naver.com</t>
+  </si>
+  <si>
+    <t>한녕균</t>
+  </si>
+  <si>
+    <t>0223wltn@naver.com</t>
+  </si>
+  <si>
+    <t>홍지수</t>
+  </si>
+  <si>
+    <t>skyhaneul0910@naver.com</t>
+  </si>
+  <si>
+    <t>권하늘</t>
+  </si>
+  <si>
+    <t>oys55736@gmail.com</t>
+  </si>
+  <si>
+    <t>오윤서</t>
+  </si>
+  <si>
+    <t>yhc0564@naver.com</t>
+  </si>
+  <si>
+    <t>윤홍채</t>
+  </si>
+  <si>
+    <t>liz030404@naver.com</t>
+  </si>
+  <si>
+    <t>이선주</t>
+  </si>
+  <si>
+    <t>wtbaa33@naver.com</t>
+  </si>
+  <si>
+    <t>김민교</t>
+  </si>
+  <si>
+    <t>ertyhx3@gmail.com</t>
+  </si>
+  <si>
+    <t>김미소</t>
+  </si>
+  <si>
+    <t>paulcho1004@naver.com</t>
+  </si>
+  <si>
+    <t>조민형</t>
+  </si>
+  <si>
+    <t>qudcksl1216@gmail.com</t>
+  </si>
+  <si>
+    <t>윤병찬</t>
+  </si>
+  <si>
+    <t>doheehana@naver.com</t>
+  </si>
+  <si>
+    <t>김도희</t>
+  </si>
+  <si>
+    <t>woosm050530@gmail.com</t>
+  </si>
+  <si>
+    <t>우수민</t>
+  </si>
+  <si>
+    <t>jmkkom@naver.com</t>
+  </si>
+  <si>
+    <t>전민균</t>
+  </si>
+  <si>
+    <t>sf12nam@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">남유정 </t>
+  </si>
+  <si>
+    <t>jungha051026@naver.com</t>
+  </si>
+  <si>
+    <t>윤정하</t>
+  </si>
+  <si>
+    <t>scott1234698@naver.com</t>
+  </si>
+  <si>
+    <t>우성진</t>
+  </si>
+  <si>
+    <t>kth4159@gmail.com</t>
+  </si>
+  <si>
+    <t>김태희</t>
+  </si>
+  <si>
+    <t>narinsong3@gmail.com</t>
+  </si>
+  <si>
+    <t>송나린</t>
+  </si>
+  <si>
+    <t>jenniferdy@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">간호학과 </t>
+  </si>
+  <si>
+    <t>권도연</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1565,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y147">
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -1483,11 +1798,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y99"/>
+  <dimension ref="A1:Y147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D154" sqref="D153:D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9137,6 +9452,3702 @@
         <v>32</v>
       </c>
     </row>
+    <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="4">
+        <v>45601.632308726854</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D100" s="5">
+        <v>20243606</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M100" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N100" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U100" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W100" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y100" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="7">
+        <v>45601.635583449075</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D101" s="8">
+        <v>20246628</v>
+      </c>
+      <c r="E101" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y101" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="4">
+        <v>45601.645942708332</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D102" s="5">
+        <v>20242503</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y102" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="7">
+        <v>45601.656595</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D103" s="8">
+        <v>20235210</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="F103" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J103" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K103" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L103" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N103" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U103" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y103" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="4">
+        <v>45601.669995555552</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" s="5">
+        <v>20227036</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y104" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="7">
+        <v>45601.674866122688</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D105" s="8">
+        <v>20217151</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y105" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="4">
+        <v>45601.694156319441</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D106" s="5">
+        <v>20246782</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y106" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="7">
+        <v>45601.695128125</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D107" s="8">
+        <v>20246780</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N107" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O107" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X107" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y107" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="4">
+        <v>45601.706411388892</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D108" s="5">
+        <v>20195170</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P108" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y108" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="7">
+        <v>45601.728916539352</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D109" s="8">
+        <v>20233060</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y109" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="4">
+        <v>45601.72974505787</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D110" s="5">
+        <v>20246302</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y110" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="7">
+        <v>45601.77266185185</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D111" s="8">
+        <v>20203213</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H111" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I111" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J111" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K111" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L111" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N111" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W111" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X111" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y111" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="4">
+        <v>45601.774930659725</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D112" s="5">
+        <v>20245246</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O112" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V112" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W112" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X112" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y112" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="7">
+        <v>45601.796591817125</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D113" s="8">
+        <v>20222359</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N113" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W113" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X113" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y113" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="4">
+        <v>45601.804950729165</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D114" s="5">
+        <v>20243065</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q114" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U114" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W114" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X114" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y114" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="7">
+        <v>45601.811363969908</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D115" s="8">
+        <v>20242518</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X115" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y115" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="4">
+        <v>45601.823880787037</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D116" s="5">
+        <v>20212801</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y116" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="7">
+        <v>45601.824826018521</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D117" s="8">
+        <v>20202817</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P117" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q117" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R117" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S117" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T117" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U117" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V117" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W117" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X117" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y117" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="4">
+        <v>45601.843265358795</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D118" s="5">
+        <v>20246241</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N118" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R118" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U118" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V118" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y118" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="7">
+        <v>45601.843748078703</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D119" s="8">
+        <v>20243813</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I119" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J119" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K119" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L119" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N119" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P119" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q119" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T119" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X119" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y119" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="4">
+        <v>45601.85635746528</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D120" s="5">
+        <v>20243829</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P120" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q120" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R120" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S120" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T120" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U120" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V120" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W120" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X120" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y120" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="7">
+        <v>45601.870281793977</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" s="8">
+        <v>20244120</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L121" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M121" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O121" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q121" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W121" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X121" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y121" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="4">
+        <v>45601.881217349539</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D122" s="5">
+        <v>20193508</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y122" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="7">
+        <v>45601.88206668981</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D123" s="8">
+        <v>20246251</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P123" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X123" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y123" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="4">
+        <v>45601.886119861112</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D124" s="5">
+        <v>20202706</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N124" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O124" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q124" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S124" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y124" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="125" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="7">
+        <v>45601.891516782409</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D125" s="8">
+        <v>20242411</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X125" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y125" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="126" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="13">
+        <v>45601.893246678243</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D126" s="14">
+        <v>20242428</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F126" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G126" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H126" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I126" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J126" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K126" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L126" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M126" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N126" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O126" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="U126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="V126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="W126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="X126" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y126" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="127" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="7">
+        <v>45601.92076734954</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D127" s="8">
+        <v>20246631</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O127" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q127" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X127" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y127" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="128" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A128" s="4">
+        <v>45601.922805624999</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D128" s="5">
+        <v>20246282</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O128" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P128" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q128" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T128" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X128" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y128" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A129" s="7">
+        <v>45601.924825462964</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D129" s="8">
+        <v>20193010</v>
+      </c>
+      <c r="E129" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O129" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P129" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X129" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y129" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A130" s="4">
+        <v>45601.938436041666</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D130" s="5">
+        <v>20243850</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K130" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M130" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N130" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P130" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q130" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R130" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S130" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X130" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y130" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="7">
+        <v>45601.976699212959</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D131" s="8">
+        <v>20243803</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="F131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O131" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y131" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="4">
+        <v>45601.981116516203</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D132" s="5">
+        <v>20242332</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N132" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O132" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q132" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R132" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W132" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X132" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y132" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A133" s="7">
+        <v>45602.015673969909</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D133" s="8">
+        <v>20192931</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G133" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H133" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I133" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J133" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K133" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L133" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M133" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N133" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O133" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X133" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y133" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="4">
+        <v>45602.049239456013</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D134" s="5">
+        <v>20243237</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P134" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y134" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="7">
+        <v>45602.061079965279</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D135" s="8">
+        <v>20241605</v>
+      </c>
+      <c r="E135" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N135" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O135" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q135" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V135" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W135" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y135" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A136" s="4">
+        <v>45602.06829625</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D136" s="5">
+        <v>20242607</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y136" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A137" s="7">
+        <v>45602.417939930558</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D137" s="8">
+        <v>20193836</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="F137" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G137" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H137" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I137" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J137" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K137" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L137" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M137" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N137" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O137" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P137" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q137" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R137" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S137" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T137" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U137" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V137" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W137" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="X137" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y137" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A138" s="4">
+        <v>45602.422074375005</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D138" s="5">
+        <v>20192926</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J138" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M138" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N138" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y138" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A139" s="7">
+        <v>45602.424043587962</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D139" s="8">
+        <v>20246215</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="F139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G139" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H139" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M139" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N139" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O139" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q139" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S139" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T139" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X139" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y139" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A140" s="4">
+        <v>45602.476880891205</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D140" s="5">
+        <v>20243630</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X140" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y140" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="7">
+        <v>45602.507631805551</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D141" s="8">
+        <v>20203425</v>
+      </c>
+      <c r="E141" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O141" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P141" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X141" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y141" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="4">
+        <v>45602.5284019213</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D142" s="5">
+        <v>20233716</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O142" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R142" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X142" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y142" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A143" s="7">
+        <v>45602.543921527773</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D143" s="8">
+        <v>20245213</v>
+      </c>
+      <c r="E143" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="F143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O143" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X143" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y143" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="4">
+        <v>45602.545268032409</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D144" s="5">
+        <v>20246633</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X144" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y144" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="7">
+        <v>45602.562701990741</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D145" s="8">
+        <v>20246230</v>
+      </c>
+      <c r="E145" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="F145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K145" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L145" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O145" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X145" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y145" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="4">
+        <v>45602.574898530089</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D146" s="5">
+        <v>20246248</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K146" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L146" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N146" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O146" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q146" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R146" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W146" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X146" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y146" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A147" s="16">
+        <v>45602.639858310184</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="D147" s="17">
+        <v>20246206</v>
+      </c>
+      <c r="E147" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="F147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O147" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="S147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="U147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="V147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="W147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X147" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y147" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BFI, MI, 241111 added
</commit_message>
<xml_diff>
--- a/R/data/food_plan_241104.xlsx
+++ b/R/data/food_plan_241104.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1B3B53-4187-4E42-9FC9-9E875C81F8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBE5640-4CB5-134F-8B33-29E97F8B7B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8305" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8972" uniqueCount="891">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2510,6 +2510,189 @@
   </si>
   <si>
     <t>서민아</t>
+  </si>
+  <si>
+    <t>lc990728@naver.com</t>
+  </si>
+  <si>
+    <t>이하은</t>
+  </si>
+  <si>
+    <t>0214lily@naver.com</t>
+  </si>
+  <si>
+    <t>김가희</t>
+  </si>
+  <si>
+    <t>zzun1414@naver.com</t>
+  </si>
+  <si>
+    <t>반도체·디스플레이스쿨</t>
+  </si>
+  <si>
+    <t>황준영</t>
+  </si>
+  <si>
+    <t>yeonjej51@gmail.com</t>
+  </si>
+  <si>
+    <t>정연제</t>
+  </si>
+  <si>
+    <t>chetbaker22@naver.com</t>
+  </si>
+  <si>
+    <t>김채원</t>
+  </si>
+  <si>
+    <t>jsh050906@naver.com</t>
+  </si>
+  <si>
+    <t>정송희</t>
+  </si>
+  <si>
+    <t>r67890@naver.com</t>
+  </si>
+  <si>
+    <t>이규형</t>
+  </si>
+  <si>
+    <t>xormr1505@naver.com</t>
+  </si>
+  <si>
+    <t>박찬원</t>
+  </si>
+  <si>
+    <t>leeeunbi0717@naver.com</t>
+  </si>
+  <si>
+    <t>이은비</t>
+  </si>
+  <si>
+    <t>seungye04@naver.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어</t>
+  </si>
+  <si>
+    <t>정승예</t>
+  </si>
+  <si>
+    <t>ksfu03@naver.com</t>
+  </si>
+  <si>
+    <t>이규성</t>
+  </si>
+  <si>
+    <t>woonsuck0916@naver.com</t>
+  </si>
+  <si>
+    <t>스마트IoT</t>
+  </si>
+  <si>
+    <t>운석현</t>
+  </si>
+  <si>
+    <t>jione0831@naver.com</t>
+  </si>
+  <si>
+    <t>윤지원</t>
+  </si>
+  <si>
+    <t>altigerlee@gmail.com</t>
+  </si>
+  <si>
+    <t>이재현</t>
+  </si>
+  <si>
+    <t>kyj57980@gmail.com</t>
+  </si>
+  <si>
+    <t>김예진</t>
+  </si>
+  <si>
+    <t>jin050828@gmail.com</t>
+  </si>
+  <si>
+    <t>김진영</t>
+  </si>
+  <si>
+    <t>erang051216@naver.com</t>
+  </si>
+  <si>
+    <t>박이랑</t>
+  </si>
+  <si>
+    <t>rer220@naver.com</t>
+  </si>
+  <si>
+    <t>김대명</t>
+  </si>
+  <si>
+    <t>tidlswjddms@naver.com</t>
+  </si>
+  <si>
+    <t>임정은</t>
+  </si>
+  <si>
+    <t>minwl19@naver.com</t>
+  </si>
+  <si>
+    <t>조민지</t>
+  </si>
+  <si>
+    <t>mi88368836@gmail.com</t>
+  </si>
+  <si>
+    <t>신민서</t>
+  </si>
+  <si>
+    <t>chsmdfur123@naver.com</t>
+  </si>
+  <si>
+    <t>금융재무</t>
+  </si>
+  <si>
+    <t>이한얼</t>
+  </si>
+  <si>
+    <t>kjins1234@naver.com</t>
+  </si>
+  <si>
+    <t>김진수</t>
+  </si>
+  <si>
+    <t>orientfun@gmail.com</t>
+  </si>
+  <si>
+    <t>이동화</t>
+  </si>
+  <si>
+    <t>haksun0217@naver.com</t>
+  </si>
+  <si>
+    <t>김학선</t>
+  </si>
+  <si>
+    <t>sin50407899@gmail.com</t>
+  </si>
+  <si>
+    <t>신재화</t>
+  </si>
+  <si>
+    <t>whdudgus1013@gmail.com</t>
+  </si>
+  <si>
+    <t>조영현</t>
+  </si>
+  <si>
+    <t>lg01022928122@gmail.com</t>
+  </si>
+  <si>
+    <t>권주용</t>
+  </si>
+  <si>
+    <t>mani4262421@naver.com</t>
   </si>
 </sst>
 </file>
@@ -2924,7 +3107,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y361">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y390">
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3157,11 +3340,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y361"/>
+  <dimension ref="A1:Y390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C368" sqref="C368"/>
+      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B397" sqref="B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30985,6 +31168,2239 @@
         <v>33</v>
       </c>
     </row>
+    <row r="362" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A362" s="4">
+        <v>45607.012796574076</v>
+      </c>
+      <c r="B362" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="C362" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D362" s="5">
+        <v>20245233</v>
+      </c>
+      <c r="E362" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="F362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G362" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H362" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N362" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O362" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W362" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X362" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y362" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="363" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A363" s="7">
+        <v>45607.019177581024</v>
+      </c>
+      <c r="B363" s="8" t="s">
+        <v>832</v>
+      </c>
+      <c r="C363" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D363" s="8">
+        <v>20214104</v>
+      </c>
+      <c r="E363" s="8" t="s">
+        <v>833</v>
+      </c>
+      <c r="F363" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K363" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O363" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X363" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y363" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="364" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A364" s="4">
+        <v>45607.068275543978</v>
+      </c>
+      <c r="B364" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="C364" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="D364" s="5">
+        <v>20203352</v>
+      </c>
+      <c r="E364" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="F364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G364" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M364" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N364" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O364" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P364" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q364" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R364" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S364" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T364" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U364" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V364" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W364" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X364" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y364" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="365" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A365" s="7">
+        <v>45607.122863784723</v>
+      </c>
+      <c r="B365" s="8" t="s">
+        <v>837</v>
+      </c>
+      <c r="C365" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D365" s="8">
+        <v>20241234</v>
+      </c>
+      <c r="E365" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="F365" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G365" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H365" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I365" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J365" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K365" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L365" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M365" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N365" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O365" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R365" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V365" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X365" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y365" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="366" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A366" s="4">
+        <v>45607.573002314813</v>
+      </c>
+      <c r="B366" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="C366" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="D366" s="5">
+        <v>20201031</v>
+      </c>
+      <c r="E366" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="F366" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K366" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O366" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y366" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="367" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A367" s="7">
+        <v>45607.580218472227</v>
+      </c>
+      <c r="B367" s="8" t="s">
+        <v>841</v>
+      </c>
+      <c r="C367" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D367" s="8">
+        <v>20243032</v>
+      </c>
+      <c r="E367" s="8" t="s">
+        <v>842</v>
+      </c>
+      <c r="F367" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G367" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H367" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I367" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J367" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K367" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L367" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M367" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N367" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O367" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P367" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q367" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R367" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S367" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T367" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U367" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V367" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W367" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X367" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y367" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="368" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A368" s="4">
+        <v>45607.595790694446</v>
+      </c>
+      <c r="B368" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="C368" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="D368" s="5">
+        <v>20205217</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="F368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K368" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L368" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M368" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N368" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O368" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P368" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q368" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R368" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S368" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T368" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U368" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V368" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W368" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X368" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y368" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="369" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A369" s="7">
+        <v>45607.632247094909</v>
+      </c>
+      <c r="B369" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="C369" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D369" s="8">
+        <v>20205176</v>
+      </c>
+      <c r="E369" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="F369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O369" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X369" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y369" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="370" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A370" s="4">
+        <v>45607.647828518515</v>
+      </c>
+      <c r="B370" s="5" t="s">
+        <v>847</v>
+      </c>
+      <c r="C370" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D370" s="5">
+        <v>20242340</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="F370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G370" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L370" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M370" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N370" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O370" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P370" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q370" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R370" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S370" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T370" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U370" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V370" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W370" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X370" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y370" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="371" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A371" s="7">
+        <v>45607.656308333331</v>
+      </c>
+      <c r="B371" s="8" t="s">
+        <v>849</v>
+      </c>
+      <c r="C371" s="8" t="s">
+        <v>850</v>
+      </c>
+      <c r="D371" s="8">
+        <v>20233846</v>
+      </c>
+      <c r="E371" s="8" t="s">
+        <v>851</v>
+      </c>
+      <c r="F371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H371" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L371" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M371" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N371" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O371" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P371" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V371" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W371" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X371" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y371" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="372" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A372" s="4">
+        <v>45607.694642870367</v>
+      </c>
+      <c r="B372" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="C372" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D372" s="5">
+        <v>20201071</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="F372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P372" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q372" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R372" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S372" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T372" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U372" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V372" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W372" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X372" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y372" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="373" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A373" s="7">
+        <v>45607.6956134375</v>
+      </c>
+      <c r="B373" s="8" t="s">
+        <v>854</v>
+      </c>
+      <c r="C373" s="8" t="s">
+        <v>855</v>
+      </c>
+      <c r="D373" s="8">
+        <v>20205206</v>
+      </c>
+      <c r="E373" s="8" t="s">
+        <v>856</v>
+      </c>
+      <c r="F373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G373" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H373" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M373" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N373" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O373" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P373" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q373" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R373" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S373" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T373" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U373" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V373" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W373" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="X373" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y373" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="374" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A374" s="4">
+        <v>45607.785850335647</v>
+      </c>
+      <c r="B374" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="C374" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D374" s="5">
+        <v>20246262</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="F374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J374" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M374" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N374" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q374" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W374" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X374" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y374" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="375" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A375" s="7">
+        <v>45607.794722395833</v>
+      </c>
+      <c r="B375" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="C375" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="D375" s="8">
+        <v>20196523</v>
+      </c>
+      <c r="E375" s="8" t="s">
+        <v>860</v>
+      </c>
+      <c r="F375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K375" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L375" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M375" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N375" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O375" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X375" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y375" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="376" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A376" s="4">
+        <v>45607.819049537036</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D376" s="5">
+        <v>20202319</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="F376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W376" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X376" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y376" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="377" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A377" s="7">
+        <v>45607.824856736115</v>
+      </c>
+      <c r="B377" s="8" t="s">
+        <v>863</v>
+      </c>
+      <c r="C377" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D377" s="8">
+        <v>20246715</v>
+      </c>
+      <c r="E377" s="8" t="s">
+        <v>864</v>
+      </c>
+      <c r="F377" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G377" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H377" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I377" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J377" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K377" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L377" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M377" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N377" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O377" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P377" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q377" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R377" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S377" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T377" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U377" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V377" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W377" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X377" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y377" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="378" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A378" s="4">
+        <v>45607.83888625</v>
+      </c>
+      <c r="B378" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="C378" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D378" s="5">
+        <v>20243223</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="F378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H378" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J378" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K378" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M378" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N378" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q378" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U378" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X378" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y378" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="379" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A379" s="7">
+        <v>45607.934080914347</v>
+      </c>
+      <c r="B379" s="8" t="s">
+        <v>867</v>
+      </c>
+      <c r="C379" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D379" s="8">
+        <v>20205124</v>
+      </c>
+      <c r="E379" s="8" t="s">
+        <v>868</v>
+      </c>
+      <c r="F379" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G379" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H379" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I379" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J379" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K379" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L379" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M379" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N379" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O379" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W379" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X379" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y379" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="380" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A380" s="4">
+        <v>45607.960547499999</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="D380" s="5">
+        <v>20205240</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="F380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y380" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="381" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A381" s="7">
+        <v>45608.013746620374</v>
+      </c>
+      <c r="B381" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="C381" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D381" s="8">
+        <v>20217178</v>
+      </c>
+      <c r="E381" s="8" t="s">
+        <v>872</v>
+      </c>
+      <c r="F381" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O381" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X381" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y381" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="382" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A382" s="4">
+        <v>45608.03375239583</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>873</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D382" s="5">
+        <v>20244126</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H382" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I382" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J382" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K382" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L382" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M382" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N382" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O382" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X382" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y382" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="383" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A383" s="7">
+        <v>45608.440838634255</v>
+      </c>
+      <c r="B383" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="C383" s="8" t="s">
+        <v>876</v>
+      </c>
+      <c r="D383" s="8">
+        <v>20203026</v>
+      </c>
+      <c r="E383" s="8" t="s">
+        <v>877</v>
+      </c>
+      <c r="F383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K383" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M383" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N383" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O383" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X383" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y383" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="384" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A384" s="4">
+        <v>45608.493099502317</v>
+      </c>
+      <c r="B384" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D384" s="5">
+        <v>20182845</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="F384" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H384" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I384" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M384" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N384" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P384" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q384" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R384" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S384" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T384" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U384" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V384" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W384" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X384" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y384" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="385" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A385" s="7">
+        <v>45608.549287152782</v>
+      </c>
+      <c r="B385" s="8" t="s">
+        <v>880</v>
+      </c>
+      <c r="C385" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D385" s="8">
+        <v>20245218</v>
+      </c>
+      <c r="E385" s="8" t="s">
+        <v>881</v>
+      </c>
+      <c r="F385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O385" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X385" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y385" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="386" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A386" s="4">
+        <v>45608.553584849535</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="C386" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D386" s="5">
+        <v>20243814</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="F386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K386" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L386" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X386" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y386" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="387" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A387" s="7">
+        <v>45608.579702662042</v>
+      </c>
+      <c r="B387" s="8" t="s">
+        <v>884</v>
+      </c>
+      <c r="C387" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D387" s="8">
+        <v>20202538</v>
+      </c>
+      <c r="E387" s="8" t="s">
+        <v>885</v>
+      </c>
+      <c r="F387" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G387" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H387" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N387" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O387" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q387" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X387" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y387" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="388" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A388" s="4">
+        <v>45608.629903796296</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D388" s="5">
+        <v>20243253</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="F388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J388" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M388" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N388" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P388" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q388" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R388" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S388" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T388" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U388" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V388" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W388" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X388" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y388" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="389" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A389" s="7">
+        <v>45608.644307071758</v>
+      </c>
+      <c r="B389" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="C389" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D389" s="8">
+        <v>20215109</v>
+      </c>
+      <c r="E389" s="8" t="s">
+        <v>889</v>
+      </c>
+      <c r="F389" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G389" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H389" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I389" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J389" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K389" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L389" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M389" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N389" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O389" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T389" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W389" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X389" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y389" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="390" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A390" s="13">
+        <v>45608.658920648144</v>
+      </c>
+      <c r="B390" s="14" t="s">
+        <v>890</v>
+      </c>
+      <c r="C390" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D390" s="14">
+        <v>20223022</v>
+      </c>
+      <c r="E390" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="F390" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G390" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H390" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I390" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J390" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K390" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L390" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M390" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N390" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O390" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q390" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="R390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="U390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="V390" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="W390" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="X390" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y390" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BFI, MI, 241111 modified 4
</commit_message>
<xml_diff>
--- a/R/data/food_plan_241104.xlsx
+++ b/R/data/food_plan_241104.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBE5640-4CB5-134F-8B33-29E97F8B7B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ED5605-A0B8-184F-9918-249F69A8BA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="1360" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8972" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9961" uniqueCount="979">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2693,6 +2693,270 @@
   </si>
   <si>
     <t>mani4262421@naver.com</t>
+  </si>
+  <si>
+    <t>smartcindyya@gmail.com</t>
+  </si>
+  <si>
+    <t>박지현</t>
+  </si>
+  <si>
+    <t>qwe92517@gmail.com</t>
+  </si>
+  <si>
+    <t>이진영</t>
+  </si>
+  <si>
+    <t>minkyoung961@naver.com</t>
+  </si>
+  <si>
+    <t>phc5120@naver.com</t>
+  </si>
+  <si>
+    <t>박희철</t>
+  </si>
+  <si>
+    <t>dongkyo4@gmail.com</t>
+  </si>
+  <si>
+    <t>이동교</t>
+  </si>
+  <si>
+    <t>xodet0817@naver.com</t>
+  </si>
+  <si>
+    <t>문종윤</t>
+  </si>
+  <si>
+    <t>ljy46tkd@naver.com</t>
+  </si>
+  <si>
+    <t>이정연</t>
+  </si>
+  <si>
+    <t>gee30901@naver.com</t>
+  </si>
+  <si>
+    <t>박예원</t>
+  </si>
+  <si>
+    <t>dw060419@naver.com</t>
+  </si>
+  <si>
+    <t>김도원</t>
+  </si>
+  <si>
+    <t>sky0219msh@naver.com</t>
+  </si>
+  <si>
+    <t>최하늘</t>
+  </si>
+  <si>
+    <t>smsong1036@gmail.com</t>
+  </si>
+  <si>
+    <t>송승민</t>
+  </si>
+  <si>
+    <t>ella2005710@gmail.com</t>
+  </si>
+  <si>
+    <t>김송이</t>
+  </si>
+  <si>
+    <t>ssjm9652@naver.com</t>
+  </si>
+  <si>
+    <t>소정민</t>
+  </si>
+  <si>
+    <t>mik21366@naver.com</t>
+  </si>
+  <si>
+    <t>김수진</t>
+  </si>
+  <si>
+    <t>kangyein0810@gmail.com</t>
+  </si>
+  <si>
+    <t>강예인</t>
+  </si>
+  <si>
+    <t>sejun4@naver.com</t>
+  </si>
+  <si>
+    <t>경영/청각</t>
+  </si>
+  <si>
+    <t>박세준</t>
+  </si>
+  <si>
+    <t>leejiheoen450@naver.com</t>
+  </si>
+  <si>
+    <t>이지현</t>
+  </si>
+  <si>
+    <t>gchans0524@gmail.com</t>
+  </si>
+  <si>
+    <t>한기찬</t>
+  </si>
+  <si>
+    <t>fred0203@naver.com</t>
+  </si>
+  <si>
+    <t>언어청각학부 청각학전공</t>
+  </si>
+  <si>
+    <t>이강준</t>
+  </si>
+  <si>
+    <t>sssm08155@gmail.com</t>
+  </si>
+  <si>
+    <t>윤희주</t>
+  </si>
+  <si>
+    <t>tqwquqqi@naver.com</t>
+  </si>
+  <si>
+    <t>강하늘</t>
+  </si>
+  <si>
+    <t>wjdalsrb303@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">정치행정학과 </t>
+  </si>
+  <si>
+    <t>정민규</t>
+  </si>
+  <si>
+    <t>kimhemi05@gmail.com</t>
+  </si>
+  <si>
+    <t>김혜미</t>
+  </si>
+  <si>
+    <t>nwjcq14@naver.com</t>
+  </si>
+  <si>
+    <t>임미정</t>
+  </si>
+  <si>
+    <t>sengyu0805@gmail.com</t>
+  </si>
+  <si>
+    <t>나선아</t>
+  </si>
+  <si>
+    <t>hyerujys2005@naver.com</t>
+  </si>
+  <si>
+    <t>정윤수</t>
+  </si>
+  <si>
+    <t>bjw2934@naver.com</t>
+  </si>
+  <si>
+    <t>방정우</t>
+  </si>
+  <si>
+    <t>kwakmin427@gmail.com</t>
+  </si>
+  <si>
+    <t>곽민규</t>
+  </si>
+  <si>
+    <t>min010417@gmail.com</t>
+  </si>
+  <si>
+    <t>강채민</t>
+  </si>
+  <si>
+    <t>wendy040507@naver.com</t>
+  </si>
+  <si>
+    <t>이수빈</t>
+  </si>
+  <si>
+    <t>jhry0903@naver.com</t>
+  </si>
+  <si>
+    <t>조하령</t>
+  </si>
+  <si>
+    <t>ksong1210@icloud.com</t>
+  </si>
+  <si>
+    <t>곽송</t>
+  </si>
+  <si>
+    <t>marlboroe53@naver.com</t>
+  </si>
+  <si>
+    <t>benjamin27@naver.com</t>
+  </si>
+  <si>
+    <t>최재혁</t>
+  </si>
+  <si>
+    <t>lsd5741@naver.com</t>
+  </si>
+  <si>
+    <t>이소담</t>
+  </si>
+  <si>
+    <t>choyunjae2153@gmail.com</t>
+  </si>
+  <si>
+    <t>AI의료융합학과</t>
+  </si>
+  <si>
+    <t>조윤재</t>
+  </si>
+  <si>
+    <t>namjihk@gmail.com</t>
+  </si>
+  <si>
+    <t>남지혁</t>
+  </si>
+  <si>
+    <t>gyucheol0503@naver.com</t>
+  </si>
+  <si>
+    <t>홍규철</t>
+  </si>
+  <si>
+    <t>qotnqls1126@naver.com</t>
+  </si>
+  <si>
+    <t>배수빈</t>
+  </si>
+  <si>
+    <t>rhkddyd234@naver.com</t>
+  </si>
+  <si>
+    <t>이광용</t>
+  </si>
+  <si>
+    <t>yeonju455@naver.com</t>
+  </si>
+  <si>
+    <t>정연주</t>
+  </si>
+  <si>
+    <t>hihi2679@gmail.com</t>
+  </si>
+  <si>
+    <t>박서현</t>
+  </si>
+  <si>
+    <t>hyeonse0@naver.com</t>
+  </si>
+  <si>
+    <t>황현서</t>
   </si>
 </sst>
 </file>
@@ -3107,7 +3371,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y390">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Y433">
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3340,11 +3604,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y390"/>
+  <dimension ref="A1:Y433"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B397" sqref="B397"/>
+      <pane ySplit="1" topLeftCell="A384" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C436" sqref="C436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33401,6 +33665,3317 @@
         <v>33</v>
       </c>
     </row>
+    <row r="391" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A391" s="7">
+        <v>45608.672256307866</v>
+      </c>
+      <c r="B391" s="8" t="s">
+        <v>891</v>
+      </c>
+      <c r="C391" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D391" s="8">
+        <v>20245172</v>
+      </c>
+      <c r="E391" s="8" t="s">
+        <v>892</v>
+      </c>
+      <c r="F391" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G391" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M391" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N391" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O391" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X391" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y391" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="392" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A392" s="4">
+        <v>45608.676491597224</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D392" s="5">
+        <v>20246271</v>
+      </c>
+      <c r="E392" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="F392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M392" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O392" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P392" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R392" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W392" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X392" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y392" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="393" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A393" s="7">
+        <v>45608.684051284727</v>
+      </c>
+      <c r="B393" s="8" t="s">
+        <v>895</v>
+      </c>
+      <c r="C393" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D393" s="8">
+        <v>20231706</v>
+      </c>
+      <c r="E393" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="F393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J393" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O393" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q393" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X393" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y393" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="394" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A394" s="4">
+        <v>45608.694012719905</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D394" s="5">
+        <v>20183824</v>
+      </c>
+      <c r="E394" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="F394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J394" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K394" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L394" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X394" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y394" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="395" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A395" s="7">
+        <v>45608.821700486107</v>
+      </c>
+      <c r="B395" s="8" t="s">
+        <v>898</v>
+      </c>
+      <c r="C395" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="D395" s="8">
+        <v>20213241</v>
+      </c>
+      <c r="E395" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="F395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J395" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K395" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O395" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P395" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q395" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U395" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X395" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y395" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="396" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A396" s="4">
+        <v>45608.852703842596</v>
+      </c>
+      <c r="B396" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="C396" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D396" s="5">
+        <v>20203616</v>
+      </c>
+      <c r="E396" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P396" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q396" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X396" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y396" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="397" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A397" s="7">
+        <v>45608.855727951392</v>
+      </c>
+      <c r="B397" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C397" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D397" s="8">
+        <v>20242737</v>
+      </c>
+      <c r="E397" s="8" t="s">
+        <v>903</v>
+      </c>
+      <c r="F397" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G397" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H397" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I397" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J397" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K397" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L397" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M397" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N397" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O397" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q397" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V397" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W397" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X397" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y397" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="398" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A398" s="4">
+        <v>45608.861882164347</v>
+      </c>
+      <c r="B398" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="C398" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D398" s="5">
+        <v>20246238</v>
+      </c>
+      <c r="E398" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="F398" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I398" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J398" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K398" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O398" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P398" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q398" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R398" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S398" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T398" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U398" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V398" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W398" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X398" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y398" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="399" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A399" s="7">
+        <v>45608.903230821757</v>
+      </c>
+      <c r="B399" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="C399" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D399" s="8">
+        <v>20241509</v>
+      </c>
+      <c r="E399" s="8" t="s">
+        <v>907</v>
+      </c>
+      <c r="F399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O399" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X399" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y399" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="400" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A400" s="4">
+        <v>45608.912203194443</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D400" s="5">
+        <v>20201108</v>
+      </c>
+      <c r="E400" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="F400" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G400" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H400" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I400" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J400" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K400" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L400" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M400" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N400" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O400" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X400" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y400" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="401" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A401" s="7">
+        <v>45608.954747523152</v>
+      </c>
+      <c r="B401" s="8" t="s">
+        <v>910</v>
+      </c>
+      <c r="C401" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="D401" s="8">
+        <v>20243624</v>
+      </c>
+      <c r="E401" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="F401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K401" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L401" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M401" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N401" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O401" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X401" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y401" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="402" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A402" s="4">
+        <v>45608.96850949074</v>
+      </c>
+      <c r="B402" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="C402" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D402" s="5">
+        <v>20246222</v>
+      </c>
+      <c r="E402" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="F402" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G402" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H402" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I402" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J402" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K402" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L402" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M402" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N402" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O402" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W402" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X402" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y402" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="403" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A403" s="7">
+        <v>45609.016103275462</v>
+      </c>
+      <c r="B403" s="8" t="s">
+        <v>914</v>
+      </c>
+      <c r="C403" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D403" s="8">
+        <v>20241047</v>
+      </c>
+      <c r="E403" s="8" t="s">
+        <v>915</v>
+      </c>
+      <c r="F403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G403" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N403" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O403" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P403" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R403" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X403" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y403" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="404" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A404" s="4">
+        <v>45609.019534212959</v>
+      </c>
+      <c r="B404" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D404" s="5">
+        <v>20233808</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="F404" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H404" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M404" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N404" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O404" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S404" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T404" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X404" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y404" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="405" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A405" s="16">
+        <v>45609.038033032411</v>
+      </c>
+      <c r="B405" s="17" t="s">
+        <v>918</v>
+      </c>
+      <c r="C405" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="D405" s="17">
+        <v>20246603</v>
+      </c>
+      <c r="E405" s="17" t="s">
+        <v>919</v>
+      </c>
+      <c r="F405" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G405" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H405" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I405" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J405" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K405" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L405" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M405" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N405" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O405" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P405" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q405" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="R405" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="S405" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="T405" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="U405" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="V405" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="W405" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="X405" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y405" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="406" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A406" s="4">
+        <v>45609.43347635417</v>
+      </c>
+      <c r="B406" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C406" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="D406" s="5">
+        <v>20193968</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="F406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O406" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X406" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y406" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="407" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A407" s="7">
+        <v>45609.46456743055</v>
+      </c>
+      <c r="B407" s="8" t="s">
+        <v>923</v>
+      </c>
+      <c r="C407" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D407" s="8">
+        <v>20242232</v>
+      </c>
+      <c r="E407" s="8" t="s">
+        <v>924</v>
+      </c>
+      <c r="F407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J407" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N407" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O407" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P407" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q407" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R407" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S407" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T407" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U407" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V407" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W407" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X407" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y407" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="408" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A408" s="4">
+        <v>45609.529891377315</v>
+      </c>
+      <c r="B408" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="C408" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D408" s="5">
+        <v>20244152</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="F408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I408" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L408" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M408" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O408" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X408" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y408" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="409" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A409" s="7">
+        <v>45609.538314907404</v>
+      </c>
+      <c r="B409" s="8" t="s">
+        <v>927</v>
+      </c>
+      <c r="C409" s="8" t="s">
+        <v>928</v>
+      </c>
+      <c r="D409" s="8">
+        <v>20227091</v>
+      </c>
+      <c r="E409" s="8" t="s">
+        <v>929</v>
+      </c>
+      <c r="F409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O409" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P409" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q409" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R409" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S409" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T409" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U409" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V409" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W409" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X409" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y409" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="410" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A410" s="4">
+        <v>45609.563055219907</v>
+      </c>
+      <c r="B410" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="C410" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D410" s="5">
+        <v>20201070</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="F410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L410" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O410" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X410" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y410" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="411" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A411" s="7">
+        <v>45609.569549328706</v>
+      </c>
+      <c r="B411" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="C411" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D411" s="8">
+        <v>20222905</v>
+      </c>
+      <c r="E411" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="F411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I411" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L411" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M411" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O411" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q411" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R411" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U411" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X411" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y411" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="412" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A412" s="4">
+        <v>45609.59851585648</v>
+      </c>
+      <c r="B412" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="C412" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="D412" s="5">
+        <v>20202431</v>
+      </c>
+      <c r="E412" s="5" t="s">
+        <v>936</v>
+      </c>
+      <c r="F412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O412" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X412" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y412" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="413" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A413" s="7">
+        <v>45609.60357835648</v>
+      </c>
+      <c r="B413" s="8" t="s">
+        <v>937</v>
+      </c>
+      <c r="C413" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D413" s="8">
+        <v>20242112</v>
+      </c>
+      <c r="E413" s="8" t="s">
+        <v>938</v>
+      </c>
+      <c r="F413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H413" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O413" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S413" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="T413" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U413" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X413" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y413" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="414" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A414" s="13">
+        <v>45609.672918217591</v>
+      </c>
+      <c r="B414" s="14" t="s">
+        <v>939</v>
+      </c>
+      <c r="C414" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D414" s="14">
+        <v>20216631</v>
+      </c>
+      <c r="E414" s="14" t="s">
+        <v>940</v>
+      </c>
+      <c r="F414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G414" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N414" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O414" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="R414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="S414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="U414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="V414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="W414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="X414" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y414" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="415" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A415" s="7">
+        <v>45609.790009490738</v>
+      </c>
+      <c r="B415" s="8" t="s">
+        <v>941</v>
+      </c>
+      <c r="C415" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D415" s="8">
+        <v>20245152</v>
+      </c>
+      <c r="E415" s="8" t="s">
+        <v>942</v>
+      </c>
+      <c r="F415" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H415" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O415" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P415" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q415" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X415" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y415" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="416" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A416" s="4">
+        <v>45609.819131342592</v>
+      </c>
+      <c r="B416" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="C416" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D416" s="5">
+        <v>20242575</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="F416" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L416" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M416" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N416" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R416" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U416" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W416" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X416" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y416" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="417" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A417" s="7">
+        <v>45609.911300347223</v>
+      </c>
+      <c r="B417" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="C417" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D417" s="8">
+        <v>20205182</v>
+      </c>
+      <c r="E417" s="8" t="s">
+        <v>946</v>
+      </c>
+      <c r="F417" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G417" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H417" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I417" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J417" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K417" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L417" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M417" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N417" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O417" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P417" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q417" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R417" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S417" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T417" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U417" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V417" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W417" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X417" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y417" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="418" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A418" s="4">
+        <v>45609.94776171296</v>
+      </c>
+      <c r="B418" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="C418" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D418" s="5">
+        <v>20243605</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="F418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O418" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X418" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y418" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="419" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A419" s="7">
+        <v>45609.949337511571</v>
+      </c>
+      <c r="B419" s="8" t="s">
+        <v>949</v>
+      </c>
+      <c r="C419" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D419" s="8">
+        <v>20203702</v>
+      </c>
+      <c r="E419" s="8" t="s">
+        <v>950</v>
+      </c>
+      <c r="F419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K419" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M419" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N419" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O419" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U419" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V419" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W419" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X419" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y419" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="420" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A420" s="4">
+        <v>45609.963245486113</v>
+      </c>
+      <c r="B420" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="C420" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D420" s="5">
+        <v>20243002</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I420" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L420" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N420" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O420" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X420" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y420" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="421" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A421" s="7">
+        <v>45609.967605150465</v>
+      </c>
+      <c r="B421" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="C421" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D421" s="8">
+        <v>20241097</v>
+      </c>
+      <c r="E421" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="F421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K421" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L421" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O421" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q421" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R421" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W421" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X421" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y421" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="422" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A422" s="13">
+        <v>45609.983206516205</v>
+      </c>
+      <c r="B422" s="14" t="s">
+        <v>955</v>
+      </c>
+      <c r="C422" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D422" s="14">
+        <v>20242304</v>
+      </c>
+      <c r="E422" s="14" t="s">
+        <v>956</v>
+      </c>
+      <c r="F422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I422" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O422" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q422" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R422" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="U422" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="V422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="W422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="X422" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y422" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="423" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A423" s="7">
+        <v>45610.00604680556</v>
+      </c>
+      <c r="B423" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="C423" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="D423" s="8">
+        <v>20203302</v>
+      </c>
+      <c r="E423" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="F423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O423" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X423" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y423" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="424" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A424" s="4">
+        <v>45610.042626168986</v>
+      </c>
+      <c r="B424" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="C424" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D424" s="5">
+        <v>20212583</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>959</v>
+      </c>
+      <c r="F424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O424" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y424" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="425" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A425" s="7">
+        <v>45610.452172453704</v>
+      </c>
+      <c r="B425" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="C425" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D425" s="8">
+        <v>20242225</v>
+      </c>
+      <c r="E425" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="F425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O425" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X425" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y425" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="426" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A426" s="4">
+        <v>45610.492903784718</v>
+      </c>
+      <c r="B426" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="C426" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="D426" s="5">
+        <v>20227162</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I426" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L426" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q426" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y426" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="427" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A427" s="7">
+        <v>45610.497153518518</v>
+      </c>
+      <c r="B427" s="8" t="s">
+        <v>965</v>
+      </c>
+      <c r="C427" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D427" s="8">
+        <v>20242944</v>
+      </c>
+      <c r="E427" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="F427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K427" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M427" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N427" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O427" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q427" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R427" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V427" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X427" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y427" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="428" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A428" s="4">
+        <v>45610.57144590278</v>
+      </c>
+      <c r="B428" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C428" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D428" s="5">
+        <v>20243650</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O428" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X428" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y428" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="429" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A429" s="7">
+        <v>45610.618265636571</v>
+      </c>
+      <c r="B429" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="C429" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D429" s="8">
+        <v>20203820</v>
+      </c>
+      <c r="E429" s="8" t="s">
+        <v>970</v>
+      </c>
+      <c r="F429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J429" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K429" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O429" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y429" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="430" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A430" s="4">
+        <v>45610.637915185187</v>
+      </c>
+      <c r="B430" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="C430" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D430" s="5">
+        <v>20193420</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="F430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L430" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N430" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O430" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P430" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T430" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V430" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X430" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y430" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="431" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A431" s="7">
+        <v>45610.686676747689</v>
+      </c>
+      <c r="B431" s="8" t="s">
+        <v>973</v>
+      </c>
+      <c r="C431" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D431" s="8">
+        <v>20226638</v>
+      </c>
+      <c r="E431" s="8" t="s">
+        <v>974</v>
+      </c>
+      <c r="F431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O431" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W431" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X431" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y431" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="432" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A432" s="4">
+        <v>45610.715277812502</v>
+      </c>
+      <c r="B432" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="C432" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D432" s="5">
+        <v>20243815</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="F432" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N432" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O432" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P432" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q432" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R432" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S432" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T432" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U432" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V432" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W432" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X432" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y432" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="433" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A433" s="16">
+        <v>45610.785899409719</v>
+      </c>
+      <c r="B433" s="17" t="s">
+        <v>977</v>
+      </c>
+      <c r="C433" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D433" s="17">
+        <v>20202761</v>
+      </c>
+      <c r="E433" s="17" t="s">
+        <v>978</v>
+      </c>
+      <c r="F433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O433" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="R433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="S433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="V433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="W433" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X433" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y433" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>